<commit_message>
Add routes table and  edit readme  error
</commit_message>
<xml_diff>
--- a/apiRoutes.xlsx
+++ b/apiRoutes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="20115" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+  <si>
+    <t>METHOD</t>
+  </si>
+  <si>
+    <t>INFO</t>
+  </si>
+  <si>
+    <t>ACL</t>
+  </si>
+  <si>
+    <t>PERMISSION</t>
+  </si>
   <si>
     <t>/info/{path}</t>
   </si>
@@ -24,90 +36,149 @@
     <t>GET</t>
   </si>
   <si>
+    <t>get information about a file or directory (size, mime-type, folder contents, etc)</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> read-file</t>
+  </si>
+  <si>
     <t>/upload</t>
   </si>
   <si>
     <t>POST</t>
   </si>
   <si>
+    <t>[file,path] - upload a file to path</t>
+  </si>
+  <si>
+    <t>cf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> create-file</t>
+  </si>
+  <si>
     <t>/add-folder</t>
   </si>
   <si>
+    <t>[path] - creates a directory</t>
+  </si>
+  <si>
     <t>/rename</t>
   </si>
   <si>
+    <t>[old_file_path,new_file_path]</t>
+  </si>
+  <si>
+    <t>uf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update-file</t>
+  </si>
+  <si>
     <t>/copy</t>
   </si>
   <si>
+    <t>[source,dest] - copies `source` to `destination` (files)</t>
+  </si>
+  <si>
     <t>/copy-folder</t>
   </si>
   <si>
+    <t>[source,dest] - copies `source` to `destination` (folder)</t>
+  </si>
+  <si>
     <t>/delete</t>
   </si>
   <si>
+    <t>[path] - delete a file or a folder if empty</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delete-file</t>
+  </si>
+  <si>
     <t>/force-delete</t>
   </si>
   <si>
+    <t>[path] - delete a file or a folder even if not empty</t>
+  </si>
+  <si>
     <t>/add-user</t>
   </si>
   <si>
+    <t>[username,permissions_string] - adds the user and responds with an API key</t>
+  </si>
+  <si>
+    <t>cu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> create-user</t>
+  </si>
+  <si>
     <t>/user/{username}</t>
   </si>
   <si>
+    <t>get user info (permissions)</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> read-user</t>
+  </si>
+  <si>
     <t>/users</t>
   </si>
   <si>
+    <t>get users list</t>
+  </si>
+  <si>
     <t>/update-user</t>
   </si>
   <si>
+    <t>[username,permissions_string] - update the user</t>
+  </si>
+  <si>
+    <t>uu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> update-users-permissions</t>
+  </si>
+  <si>
     <t>/delete-user</t>
   </si>
   <si>
     <t>[username] - deletes the user</t>
   </si>
   <si>
-    <t>[username,permissions_string] - update the user</t>
-  </si>
-  <si>
-    <t>get users list</t>
-  </si>
-  <si>
-    <t>get user info (permissions)</t>
-  </si>
-  <si>
-    <t>get information about a file or directory (size, mime-type, folder contents, etc)</t>
-  </si>
-  <si>
-    <t>[file,path] - upload a file to path</t>
-  </si>
-  <si>
-    <t>[path] - creates a directory</t>
-  </si>
-  <si>
-    <t>[old_file_path,new_file_path]</t>
-  </si>
-  <si>
-    <t>[source,dest] - copies `source` to `destination` (files)</t>
-  </si>
-  <si>
-    <t>[source,dest] - copies `source` to `destination` (folder)</t>
-  </si>
-  <si>
-    <t>[path] - delete a file or a folder if empty</t>
-  </si>
-  <si>
-    <t>[path] - delete a file or a folder even if not empty</t>
-  </si>
-  <si>
-    <t>[username,permissions_string] - adds the user and responds with an API key</t>
+    <t>du</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delete-user</t>
+  </si>
+  <si>
+    <t>ROUTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,8 +206,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,164 +505,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -598,7 +770,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -610,7 +782,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>